<commit_message>
Results from sim3.1 and sim3.2
</commit_message>
<xml_diff>
--- a/Simulations planning/SimPlanning.k2.p2.t10.exact_09.10.xlsx
+++ b/Simulations planning/SimPlanning.k2.p2.t10.exact_09.10.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\Simulations planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BF4C7D-4F3F-4AE7-AAAE-0FE99B9576EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFC7377-088A-446D-AEF8-0E092F581371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim0" sheetId="5" r:id="rId1"/>
     <sheet name="Sim1" sheetId="4" r:id="rId2"/>
     <sheet name="Sim2" sheetId="7" r:id="rId3"/>
-    <sheet name="Sim3" sheetId="9" r:id="rId4"/>
-    <sheet name="SimIdea1" sheetId="8" r:id="rId5"/>
-    <sheet name="Sim1_Ntotal=2000" sheetId="1" state="hidden" r:id="rId6"/>
-    <sheet name="Sim1_Ntotal=1000" sheetId="3" state="hidden" r:id="rId7"/>
-    <sheet name="Degrees of power" sheetId="2" state="hidden" r:id="rId8"/>
+    <sheet name="Sim3.1" sheetId="9" r:id="rId4"/>
+    <sheet name="Sim3.2" sheetId="11" r:id="rId5"/>
+    <sheet name="SimIdea1" sheetId="8" r:id="rId6"/>
+    <sheet name="Overview" sheetId="10" r:id="rId7"/>
+    <sheet name="Sim1_Ntotal=2000" sheetId="1" state="hidden" r:id="rId8"/>
+    <sheet name="Sim1_Ntotal=1000" sheetId="3" state="hidden" r:id="rId9"/>
+    <sheet name="Degrees of power" sheetId="2" state="hidden" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="75">
   <si>
     <t>Condition</t>
   </si>
@@ -207,13 +209,67 @@
     <t>avg.power</t>
   </si>
   <si>
-    <t>Diff.median.mean.power</t>
-  </si>
-  <si>
     <t>hypothesis</t>
   </si>
   <si>
     <t>b1&gt;b2</t>
+  </si>
+  <si>
+    <t>Manipulated</t>
+  </si>
+  <si>
+    <t>Sim1</t>
+  </si>
+  <si>
+    <t>average power of the set, given that all studies have the same power</t>
+  </si>
+  <si>
+    <t>Sim2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spread of the power in the set: sum of squares of the power levels </t>
+  </si>
+  <si>
+    <t>Simulation number</t>
+  </si>
+  <si>
+    <t>Manipulated_wording</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>Power.1</t>
+  </si>
+  <si>
+    <t>Power.2</t>
+  </si>
+  <si>
+    <t>Power.3</t>
+  </si>
+  <si>
+    <t>Power.4</t>
+  </si>
+  <si>
+    <t>Power.5</t>
+  </si>
+  <si>
+    <t>Power.6</t>
+  </si>
+  <si>
+    <t>Power.7</t>
+  </si>
+  <si>
+    <t>Power.8</t>
+  </si>
+  <si>
+    <t>Power.9</t>
+  </si>
+  <si>
+    <t>Power.10</t>
   </si>
 </sst>
 </file>
@@ -299,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -367,11 +423,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -435,7 +500,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,7 +795,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,7 +808,7 @@
         <v>46</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>47</v>
@@ -770,7 +837,7 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2">
         <v>0.3</v>
@@ -799,7 +866,7 @@
         <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>0.3</v>
@@ -828,7 +895,7 @@
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4">
         <v>0.3</v>
@@ -857,7 +924,7 @@
         <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <v>0.3</v>
@@ -886,7 +953,7 @@
         <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>0.3</v>
@@ -915,7 +982,7 @@
         <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7">
         <v>0.3</v>
@@ -944,7 +1011,7 @@
         <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8">
         <v>0.3</v>
@@ -973,7 +1040,7 @@
         <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9">
         <v>0.3</v>
@@ -1002,7 +1069,7 @@
         <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10">
         <v>0.3</v>
@@ -1031,7 +1098,7 @@
         <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="19">
         <v>0.3</v>
@@ -1059,12 +1126,234 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65C1D6A-9ED8-4638-8561-F699B52D61B5}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="11" width="14.21875" customWidth="1"/>
+    <col min="14" max="14" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="24"/>
+      <c r="I2" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3">
+        <v>300</v>
+      </c>
+      <c r="F3">
+        <v>400</v>
+      </c>
+      <c r="G3">
+        <v>500</v>
+      </c>
+      <c r="H3">
+        <v>600</v>
+      </c>
+      <c r="I3">
+        <v>700</v>
+      </c>
+      <c r="J3">
+        <v>800</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>55</v>
+      </c>
+      <c r="D14">
+        <v>104</v>
+      </c>
+      <c r="E14">
+        <v>167</v>
+      </c>
+      <c r="F14">
+        <v>257</v>
+      </c>
+      <c r="G14">
+        <v>391</v>
+      </c>
+      <c r="H14">
+        <v>586</v>
+      </c>
+      <c r="I14">
+        <v>976</v>
+      </c>
+      <c r="J14">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.5</v>
+      </c>
+      <c r="B15">
+        <v>0.6</v>
+      </c>
+      <c r="C15">
+        <v>0.65</v>
+      </c>
+      <c r="D15">
+        <v>0.7</v>
+      </c>
+      <c r="E15">
+        <v>0.75</v>
+      </c>
+      <c r="F15">
+        <v>0.8</v>
+      </c>
+      <c r="G15">
+        <v>0.85</v>
+      </c>
+      <c r="H15">
+        <v>0.9</v>
+      </c>
+      <c r="I15">
+        <v>0.95</v>
+      </c>
+      <c r="J15">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>0.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1E3F23-FB2A-4BE0-9E04-457B31D94BA1}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,7 +1401,7 @@
         <v>31</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="18" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1524,15 +1813,6 @@
       <c r="M11" s="19">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M12" s="33"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M13" s="33"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M14" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1546,7 +1826,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M6"/>
+      <selection activeCell="C10" sqref="C10:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1592,7 +1872,7 @@
         <v>31</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1603,37 +1883,37 @@
         <v>43</v>
       </c>
       <c r="C2">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="D2">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="E2">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="F2">
-        <v>160</v>
-      </c>
-      <c r="G2" s="29">
-        <v>160</v>
+        <v>415</v>
+      </c>
+      <c r="G2">
+        <v>415</v>
       </c>
       <c r="H2">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="I2">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="J2">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="K2">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="L2">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="M2" s="18">
-        <f>DEVSQ(C2:L2)</f>
+        <f>DEVSQ(0.75,0.75,0.75,0.75,0.75,0.75,0.75,0.75,0.75,0.75)</f>
         <v>0</v>
       </c>
     </row>
@@ -1645,38 +1925,38 @@
         <v>40</v>
       </c>
       <c r="C3">
-        <v>102</v>
+        <v>251</v>
       </c>
       <c r="D3">
-        <v>102</v>
+        <v>251</v>
       </c>
       <c r="E3">
-        <v>102</v>
+        <v>251</v>
       </c>
       <c r="F3">
-        <v>102</v>
-      </c>
-      <c r="G3" s="29">
-        <v>102</v>
+        <v>251</v>
+      </c>
+      <c r="G3">
+        <v>251</v>
       </c>
       <c r="H3">
-        <v>257</v>
+        <v>632</v>
       </c>
       <c r="I3">
-        <v>257</v>
+        <v>632</v>
       </c>
       <c r="J3">
-        <v>257</v>
+        <v>632</v>
       </c>
       <c r="K3">
-        <v>257</v>
+        <v>632</v>
       </c>
       <c r="L3">
-        <v>257</v>
+        <v>632</v>
       </c>
       <c r="M3" s="18">
-        <f t="shared" ref="M3:M6" si="0">DEVSQ(C3:L3)</f>
-        <v>60062.5</v>
+        <f>DEVSQ(0.7,0.7,0.7,0.7,0.7,  0.8,0.8,0.8,0.8,0.8)</f>
+        <v>2.5000000000000046E-2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1687,38 +1967,38 @@
         <v>41</v>
       </c>
       <c r="C4">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="D4">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="E4">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="F4">
-        <v>55</v>
-      </c>
-      <c r="G4" s="29">
-        <v>55</v>
+        <v>138</v>
+      </c>
+      <c r="G4">
+        <v>138</v>
       </c>
       <c r="H4">
-        <v>383</v>
+        <v>950</v>
       </c>
       <c r="I4">
-        <v>383</v>
+        <v>950</v>
       </c>
       <c r="J4">
-        <v>383</v>
+        <v>950</v>
       </c>
       <c r="K4">
-        <v>383</v>
+        <v>950</v>
       </c>
       <c r="L4">
-        <v>383</v>
+        <v>950</v>
       </c>
       <c r="M4" s="18">
-        <f t="shared" si="0"/>
-        <v>268960</v>
+        <f>DEVSQ(0.65,0.65,0.65,0.65,0.65,  0.85, 0.85, 0.85, 0.85, 0.85)</f>
+        <v>9.999999999999995E-2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1729,38 +2009,38 @@
         <v>44</v>
       </c>
       <c r="C5">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="D5">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="E5">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F5">
-        <v>27</v>
-      </c>
-      <c r="G5" s="29">
-        <v>27</v>
+        <v>65</v>
+      </c>
+      <c r="G5">
+        <v>65</v>
       </c>
       <c r="H5">
-        <v>577</v>
+        <v>65</v>
       </c>
       <c r="I5">
-        <v>577</v>
+        <v>1441</v>
       </c>
       <c r="J5">
-        <v>577</v>
+        <v>1441</v>
       </c>
       <c r="K5">
-        <v>577</v>
+        <v>1441</v>
       </c>
       <c r="L5">
-        <v>577</v>
+        <v>1441</v>
       </c>
       <c r="M5" s="18">
-        <f t="shared" si="0"/>
-        <v>756250</v>
+        <f>DEVSQ(0.6,0.6,0.6,0.6,0.6,  0.9, 0.9, 0.9, 0.9, 0.9)</f>
+        <v>0.22500000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1770,39 +2050,39 @@
       <c r="B6" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="19">
-        <v>10</v>
-      </c>
-      <c r="D6" s="19">
-        <v>10</v>
-      </c>
-      <c r="E6" s="19">
-        <v>10</v>
-      </c>
-      <c r="F6" s="19">
-        <v>10</v>
-      </c>
-      <c r="G6" s="32">
-        <v>10</v>
-      </c>
-      <c r="H6" s="19">
-        <v>925</v>
+      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>19</v>
+      </c>
+      <c r="H6">
+        <v>19</v>
       </c>
       <c r="I6" s="19">
-        <v>925</v>
+        <v>2406</v>
       </c>
       <c r="J6" s="19">
-        <v>925</v>
+        <v>2406</v>
       </c>
       <c r="K6" s="19">
-        <v>925</v>
+        <v>2406</v>
       </c>
       <c r="L6" s="19">
-        <v>925</v>
-      </c>
-      <c r="M6" s="2">
-        <f>DEVSQ(C6:L6)</f>
-        <v>2093062.5</v>
+        <v>2406</v>
+      </c>
+      <c r="M6" s="18">
+        <f>DEVSQ(0.55,0.55,0.55,0.55,0.55,  0.95, 0.95, 0.95, 0.95, 0.95)</f>
+        <v>0.3999999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1832,20 +2112,9 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="28"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
@@ -1888,10 +2157,368 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA529D7A-73F2-4FF3-A83D-DCD91E760276}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="14" max="15" width="8.88671875" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="X1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="28">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2">
+        <v>415</v>
+      </c>
+      <c r="D2">
+        <v>415</v>
+      </c>
+      <c r="E2">
+        <v>415</v>
+      </c>
+      <c r="F2">
+        <v>415</v>
+      </c>
+      <c r="G2">
+        <v>415</v>
+      </c>
+      <c r="H2">
+        <v>415</v>
+      </c>
+      <c r="I2">
+        <v>415</v>
+      </c>
+      <c r="J2">
+        <v>415</v>
+      </c>
+      <c r="K2">
+        <v>415</v>
+      </c>
+      <c r="L2">
+        <v>415</v>
+      </c>
+      <c r="M2" s="18">
+        <f>N2-O2</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="35">
+        <f>MEDIAN(P2:Y2)</f>
+        <v>0.75</v>
+      </c>
+      <c r="O2" s="33">
+        <f>AVERAGE(P2:Y2)</f>
+        <v>0.75</v>
+      </c>
+      <c r="P2">
+        <v>0.75</v>
+      </c>
+      <c r="Q2">
+        <v>0.75</v>
+      </c>
+      <c r="R2">
+        <v>0.75</v>
+      </c>
+      <c r="S2">
+        <v>0.75</v>
+      </c>
+      <c r="T2">
+        <v>0.75</v>
+      </c>
+      <c r="U2">
+        <v>0.75</v>
+      </c>
+      <c r="V2">
+        <v>0.75</v>
+      </c>
+      <c r="W2">
+        <v>0.75</v>
+      </c>
+      <c r="X2">
+        <v>0.75</v>
+      </c>
+      <c r="Y2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="28">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3">
+        <v>251</v>
+      </c>
+      <c r="D3">
+        <v>251</v>
+      </c>
+      <c r="E3">
+        <v>251</v>
+      </c>
+      <c r="F3">
+        <v>251</v>
+      </c>
+      <c r="G3">
+        <v>251</v>
+      </c>
+      <c r="H3">
+        <v>251</v>
+      </c>
+      <c r="I3">
+        <v>415</v>
+      </c>
+      <c r="J3">
+        <v>632</v>
+      </c>
+      <c r="K3">
+        <v>950</v>
+      </c>
+      <c r="L3">
+        <v>1441</v>
+      </c>
+      <c r="M3" s="18">
+        <f t="shared" ref="M3:M4" si="0">N3-O3</f>
+        <v>-5.0000000000000044E-2</v>
+      </c>
+      <c r="N3" s="35">
+        <f>MEDIAN(P3:Y3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="O3" s="33">
+        <f>AVERAGE(P3:Y3)</f>
+        <v>0.75</v>
+      </c>
+      <c r="P3">
+        <v>0.7</v>
+      </c>
+      <c r="Q3">
+        <v>0.7</v>
+      </c>
+      <c r="R3">
+        <v>0.7</v>
+      </c>
+      <c r="S3">
+        <v>0.7</v>
+      </c>
+      <c r="T3">
+        <v>0.7</v>
+      </c>
+      <c r="U3">
+        <v>0.7</v>
+      </c>
+      <c r="V3">
+        <v>0.75</v>
+      </c>
+      <c r="W3">
+        <v>0.8</v>
+      </c>
+      <c r="X3">
+        <v>0.85</v>
+      </c>
+      <c r="Y3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="28">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4">
+        <v>138</v>
+      </c>
+      <c r="D4">
+        <v>138</v>
+      </c>
+      <c r="E4">
+        <v>138</v>
+      </c>
+      <c r="F4">
+        <v>138</v>
+      </c>
+      <c r="G4">
+        <v>138</v>
+      </c>
+      <c r="H4">
+        <v>138</v>
+      </c>
+      <c r="I4">
+        <v>1441</v>
+      </c>
+      <c r="J4">
+        <v>1441</v>
+      </c>
+      <c r="K4">
+        <v>1441</v>
+      </c>
+      <c r="L4">
+        <v>1441</v>
+      </c>
+      <c r="M4" s="18">
+        <f t="shared" si="0"/>
+        <v>-0.10000000000000009</v>
+      </c>
+      <c r="N4" s="35">
+        <f t="shared" ref="N4" si="1">MEDIAN(P4:Y4)</f>
+        <v>0.65</v>
+      </c>
+      <c r="O4" s="33">
+        <f>AVERAGE(P4:Y4)</f>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="P4">
+        <v>0.65</v>
+      </c>
+      <c r="Q4">
+        <v>0.65</v>
+      </c>
+      <c r="R4">
+        <v>0.65</v>
+      </c>
+      <c r="S4">
+        <v>0.65</v>
+      </c>
+      <c r="T4">
+        <v>0.65</v>
+      </c>
+      <c r="U4">
+        <v>0.65</v>
+      </c>
+      <c r="V4">
+        <v>0.9</v>
+      </c>
+      <c r="W4">
+        <v>0.9</v>
+      </c>
+      <c r="X4">
+        <v>0.9</v>
+      </c>
+      <c r="Y4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="28"/>
+      <c r="B5" s="1"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="33"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="21"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="33"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5273A9CC-C055-45BD-A6BA-17151D0F97B7}">
+  <dimension ref="A1:Y20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1901,289 +2528,357 @@
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="M1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="X1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="28">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2">
+        <v>415</v>
+      </c>
+      <c r="D2">
+        <v>415</v>
+      </c>
+      <c r="E2">
+        <v>415</v>
+      </c>
+      <c r="F2">
+        <v>415</v>
+      </c>
+      <c r="G2">
+        <v>415</v>
+      </c>
+      <c r="H2">
+        <v>415</v>
+      </c>
+      <c r="I2">
+        <v>415</v>
+      </c>
+      <c r="J2">
+        <v>415</v>
+      </c>
+      <c r="K2">
+        <v>415</v>
+      </c>
+      <c r="L2">
+        <v>415</v>
+      </c>
+      <c r="M2" s="18">
+        <f>N2-O2</f>
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" s="34">
+        <f>MEDIAN(P2:Y2)</f>
+        <v>0.75</v>
+      </c>
+      <c r="O2" s="29">
+        <f>AVERAGE(P2:Y2)</f>
+        <v>0.75</v>
+      </c>
+      <c r="P2">
+        <v>0.75</v>
+      </c>
+      <c r="Q2">
+        <v>0.75</v>
+      </c>
+      <c r="R2">
+        <v>0.75</v>
+      </c>
+      <c r="S2">
+        <v>0.75</v>
+      </c>
+      <c r="T2">
+        <v>0.75</v>
+      </c>
+      <c r="U2">
+        <v>0.75</v>
+      </c>
+      <c r="V2">
+        <v>0.75</v>
+      </c>
+      <c r="W2">
+        <v>0.75</v>
+      </c>
+      <c r="X2">
+        <v>0.75</v>
+      </c>
+      <c r="Y2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3">
-        <v>160</v>
+        <v>65</v>
       </c>
       <c r="D3">
-        <v>160</v>
+        <v>65</v>
       </c>
       <c r="E3">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="F3">
-        <v>160</v>
-      </c>
-      <c r="G3" s="29">
-        <v>160</v>
+        <v>138</v>
+      </c>
+      <c r="G3">
+        <v>415</v>
       </c>
       <c r="H3">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="I3">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="J3">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="K3">
-        <v>160</v>
+        <v>415</v>
       </c>
       <c r="L3">
-        <v>160</v>
-      </c>
-      <c r="M3" s="18"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+      <c r="M3" s="18">
+        <f t="shared" ref="M3" si="0">N3-O3</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="N3" s="34">
+        <f>MEDIAN(P3:Y3)</f>
+        <v>0.75</v>
+      </c>
+      <c r="O3" s="29">
+        <f>AVERAGE(P3:Y3)</f>
+        <v>0.7</v>
+      </c>
+      <c r="P3">
+        <v>0.6</v>
+      </c>
+      <c r="Q3">
+        <v>0.6</v>
+      </c>
+      <c r="R3">
+        <v>0.65</v>
+      </c>
+      <c r="S3">
+        <v>0.65</v>
+      </c>
+      <c r="T3">
+        <v>0.75</v>
+      </c>
+      <c r="U3">
+        <v>0.75</v>
+      </c>
+      <c r="V3">
+        <v>0.75</v>
+      </c>
+      <c r="W3">
+        <v>0.75</v>
+      </c>
+      <c r="X3">
+        <v>0.75</v>
+      </c>
+      <c r="Y3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>102</v>
-      </c>
-      <c r="G4" s="29">
-        <v>102</v>
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>415</v>
       </c>
       <c r="H4">
-        <v>257</v>
+        <v>415</v>
       </c>
       <c r="I4">
-        <v>257</v>
+        <v>415</v>
       </c>
       <c r="J4">
-        <v>257</v>
+        <v>415</v>
       </c>
       <c r="K4">
-        <v>257</v>
+        <v>415</v>
       </c>
       <c r="L4">
-        <v>257</v>
-      </c>
-      <c r="M4" s="18"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="28">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5">
-        <v>55</v>
-      </c>
-      <c r="D5">
-        <v>55</v>
-      </c>
-      <c r="E5">
-        <v>55</v>
-      </c>
-      <c r="F5">
-        <v>55</v>
-      </c>
-      <c r="G5" s="29">
-        <v>55</v>
-      </c>
-      <c r="H5">
-        <v>383</v>
-      </c>
-      <c r="I5">
-        <v>383</v>
-      </c>
-      <c r="J5">
-        <v>383</v>
-      </c>
-      <c r="K5">
-        <v>383</v>
-      </c>
-      <c r="L5">
-        <v>383</v>
-      </c>
+        <v>415</v>
+      </c>
+      <c r="M4" s="18">
+        <f>N4-O4</f>
+        <v>8.5559999999999969E-2</v>
+      </c>
+      <c r="N4" s="34">
+        <f>MEDIAN(P4:Y4)</f>
+        <v>0.75</v>
+      </c>
+      <c r="O4" s="29">
+        <f>AVERAGE(P4:Y4)</f>
+        <v>0.66444000000000003</v>
+      </c>
+      <c r="P4">
+        <v>0.53610000000000002</v>
+      </c>
+      <c r="Q4">
+        <v>0.53610000000000002</v>
+      </c>
+      <c r="R4">
+        <v>0.53610000000000002</v>
+      </c>
+      <c r="S4">
+        <v>0.53610000000000002</v>
+      </c>
+      <c r="T4">
+        <v>0.75</v>
+      </c>
+      <c r="U4">
+        <v>0.75</v>
+      </c>
+      <c r="V4">
+        <v>0.75</v>
+      </c>
+      <c r="W4">
+        <v>0.75</v>
+      </c>
+      <c r="X4">
+        <v>0.75</v>
+      </c>
+      <c r="Y4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="28"/>
+      <c r="B5" s="1"/>
       <c r="M5" s="18"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="28">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6">
-        <v>27</v>
-      </c>
-      <c r="D6">
-        <v>27</v>
-      </c>
-      <c r="E6">
-        <v>27</v>
-      </c>
-      <c r="F6">
-        <v>27</v>
-      </c>
-      <c r="G6" s="29">
-        <v>27</v>
-      </c>
-      <c r="H6">
-        <v>577</v>
-      </c>
-      <c r="I6">
-        <v>577</v>
-      </c>
-      <c r="J6">
-        <v>577</v>
-      </c>
-      <c r="K6">
-        <v>577</v>
-      </c>
-      <c r="L6">
-        <v>577</v>
-      </c>
+      <c r="N5" s="34"/>
+      <c r="O5" s="29"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="21"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
       <c r="M6" s="18"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
-        <v>5</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="19">
-        <v>10</v>
-      </c>
-      <c r="D7" s="19">
-        <v>10</v>
-      </c>
-      <c r="E7" s="19">
-        <v>10</v>
-      </c>
-      <c r="F7" s="19">
-        <v>10</v>
-      </c>
-      <c r="G7" s="32">
-        <v>10</v>
-      </c>
-      <c r="H7" s="19">
-        <v>925</v>
-      </c>
-      <c r="I7" s="19">
-        <v>925</v>
-      </c>
-      <c r="J7" s="19">
-        <v>925</v>
-      </c>
-      <c r="K7" s="19">
-        <v>925</v>
-      </c>
-      <c r="L7" s="19">
-        <v>925</v>
-      </c>
-      <c r="M7" s="2"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="29"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C519ED-5A47-4962-8BD0-F847E7F6AFAF}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -2283,7 +2978,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63606A17-1E3F-4AAF-B7FE-D5353955BA45}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
@@ -2703,7 +3450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9070EDF0-829D-4F07-965D-C082A11BFB0B}">
   <dimension ref="A1:M10"/>
   <sheetViews>
@@ -3120,226 +3867,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65C1D6A-9ED8-4638-8561-F699B52D61B5}">
-  <dimension ref="A1:L25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="11" width="14.21875" customWidth="1"/>
-    <col min="14" max="14" width="14.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>25</v>
-      </c>
-      <c r="B3">
-        <v>50</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>200</v>
-      </c>
-      <c r="E3">
-        <v>300</v>
-      </c>
-      <c r="F3">
-        <v>400</v>
-      </c>
-      <c r="G3">
-        <v>500</v>
-      </c>
-      <c r="H3">
-        <v>600</v>
-      </c>
-      <c r="I3">
-        <v>700</v>
-      </c>
-      <c r="J3">
-        <v>800</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>27</v>
-      </c>
-      <c r="C14">
-        <v>55</v>
-      </c>
-      <c r="D14">
-        <v>104</v>
-      </c>
-      <c r="E14">
-        <v>167</v>
-      </c>
-      <c r="F14">
-        <v>257</v>
-      </c>
-      <c r="G14">
-        <v>391</v>
-      </c>
-      <c r="H14">
-        <v>586</v>
-      </c>
-      <c r="I14">
-        <v>976</v>
-      </c>
-      <c r="J14">
-        <v>1952</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>0.5</v>
-      </c>
-      <c r="B15">
-        <v>0.6</v>
-      </c>
-      <c r="C15">
-        <v>0.65</v>
-      </c>
-      <c r="D15">
-        <v>0.7</v>
-      </c>
-      <c r="E15">
-        <v>0.75</v>
-      </c>
-      <c r="F15">
-        <v>0.8</v>
-      </c>
-      <c r="G15">
-        <v>0.85</v>
-      </c>
-      <c r="H15">
-        <v>0.9</v>
-      </c>
-      <c r="I15">
-        <v>0.95</v>
-      </c>
-      <c r="J15">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L20">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="21" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L21">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L22">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="23" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L23">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="24" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L24">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="25" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L25">
-        <v>0.99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>